<commit_message>
Questões 1 e 2 da lista de regressão.
</commit_message>
<xml_diff>
--- a/regressao/ataque_cardiaco.xlsx
+++ b/regressao/ataque_cardiaco.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>Idade</t>
   </si>
@@ -65,13 +65,29 @@
   <si>
     <t>Previsto - 10 primeiros</t>
   </si>
+  <si>
+    <t>Erro</t>
+  </si>
+  <si>
+    <t>Erro quadrático médio total:</t>
+  </si>
+  <si>
+    <t>ERRO QM</t>
+  </si>
+  <si>
+    <t>Previsto - 5 pri. 5 ult.</t>
+  </si>
+  <si>
+    <t>5 primeiros e 5 últimos</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="166" formatCode="0.000000"/>
+    <numFmt numFmtId="173" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -90,7 +106,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -111,19 +127,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -134,7 +162,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -146,6 +174,21 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -242,30 +285,69 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom/>
@@ -278,9 +360,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -290,10 +370,10 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -304,9 +384,7 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -316,11 +394,11 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -329,42 +407,64 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="173" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1656,7 +1756,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Plan1!$D$1</c:f>
+              <c:f>Plan1!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1760,69 +1860,247 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Plan1!$D$2:$D$21</c:f>
+              <c:f>Plan1!$G$2:$G$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>5.3506420810009891E-2</c:v>
+                  <c:v>5.3522460594637541E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.9402041488310834E-2</c:v>
+                  <c:v>6.9477890496516814E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.529766216661179E-2</c:v>
+                  <c:v>8.5433320398396073E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.10119328284491275</c:v>
+                  <c:v>0.10138875030027533</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.11708890352321369</c:v>
+                  <c:v>0.11734418020215459</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.13298452420151466</c:v>
+                  <c:v>0.13329961010403385</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.1488801448798156</c:v>
+                  <c:v>0.14925504000591311</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.16477576555811654</c:v>
+                  <c:v>0.1652104699077924</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.18067138623641751</c:v>
+                  <c:v>0.18116589980967165</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.19656700691471846</c:v>
+                  <c:v>0.19712132971155091</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.21246262759301943</c:v>
+                  <c:v>0.21307675961343017</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.22835824827132037</c:v>
+                  <c:v>0.22903218951530943</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.24425386894962134</c:v>
+                  <c:v>0.24498761941718869</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.26014948962792228</c:v>
+                  <c:v>0.26094304931906798</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.27604511030622325</c:v>
+                  <c:v>0.27689847922094724</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.29194073098452422</c:v>
+                  <c:v>0.29285390912282649</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.32373197234112605</c:v>
+                  <c:v>0.32476476892658501</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.37141883437602896</c:v>
+                  <c:v>0.37263105863222279</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.4508969377675337</c:v>
+                  <c:v>0.45240820814161908</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.53037504115903855</c:v>
+                  <c:v>0.53218535765101538</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Plan1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Previsto - 5 pri. 5 ult.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Plan1!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>70</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Plan1!$E$2:$E$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>6.4979465240641729E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.2958288770053484E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.10093711229946525</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.11891593582887702</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.13689475935828879</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.15487358288770056</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.17285240641711233</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.19083122994652407</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.20881005347593584</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.22678887700534761</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.24476770053475938</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.26274652406417115</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.28072534759358292</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.29870417112299469</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.31668299465240646</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.33466181818181823</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.37061946524064177</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.42455593582887702</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.51445005347593586</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.60434417112299466</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3713,16 +3991,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>131916</xdr:rowOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>93816</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>161926</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>123826</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3743,16 +4021,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>161924</xdr:rowOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3773,16 +4051,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>142874</xdr:rowOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4071,10 +4349,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="N4" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="X7" sqref="X7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4082,391 +4360,792 @@
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.42578125" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" customWidth="1"/>
-    <col min="8" max="8" width="4.42578125" customWidth="1"/>
-    <col min="9" max="9" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" customWidth="1"/>
+    <col min="10" max="10" width="4.42578125" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" customWidth="1"/>
+    <col min="12" max="12" width="4.42578125" customWidth="1"/>
+    <col min="13" max="13" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="3"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="28" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12">
+    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
         <v>10</v>
       </c>
-      <c r="B2" s="17">
+      <c r="B2" s="6">
         <v>0.05</v>
       </c>
-      <c r="C2" s="20">
-        <f>$G$2+$I$2*A2</f>
+      <c r="C2" s="9">
+        <f>$K$2+$M$2*A2</f>
         <v>4.9461928934010149E-2</v>
       </c>
-      <c r="D2" s="20">
-        <f>$G$4+$I$4*A2</f>
-        <v>5.3506420810009891E-2</v>
-      </c>
-      <c r="F2" s="4" t="s">
+      <c r="D2" s="14">
+        <f>B2-C2</f>
+        <v>5.3807106598985355E-4</v>
+      </c>
+      <c r="E2" s="9">
+        <f>$K$4+$M$4*A2</f>
+        <v>6.4979465240641729E-2</v>
+      </c>
+      <c r="F2" s="12">
+        <f>B2-E2</f>
+        <v>-1.4979465240641726E-2</v>
+      </c>
+      <c r="G2" s="9">
+        <f>$K$6+$M$6*A2</f>
+        <v>5.3522460594637541E-2</v>
+      </c>
+      <c r="H2" s="12">
+        <f>C2-G2</f>
+        <v>-4.0605316606273922E-3</v>
+      </c>
+      <c r="J2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="5">
-        <f>AVERAGE(B2:B11)-I2*AVERAGE(A2:A11)</f>
+      <c r="K2" s="29">
+        <f>AVERAGE(B2:B11)-M2*AVERAGE(A2:A11)</f>
         <v>1.0862944162436522E-3</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="L2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="8">
+      <c r="M2" s="24">
         <f>SUMPRODUCT(A2:A11,B2:B11)/SUMSQ(A2:A11)</f>
         <v>4.8375634517766495E-3</v>
       </c>
+      <c r="N2" s="30">
+        <f>SUMSQ(D2:D11)</f>
+        <v>4.8424025354943566E-4</v>
+      </c>
+      <c r="O2" s="31">
+        <f>SUMSQ(D12:D21)</f>
+        <v>0.34135980519982478</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="12">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
         <v>12</v>
       </c>
-      <c r="B3" s="17">
+      <c r="B3" s="6">
         <v>0.06</v>
       </c>
-      <c r="C3" s="20">
-        <f t="shared" ref="C3:C21" si="0">$G$2+$I$2*A3</f>
+      <c r="C3" s="9">
+        <f t="shared" ref="C3:C21" si="0">$K$2+$M$2*A3</f>
         <v>5.9137055837563443E-2</v>
       </c>
-      <c r="D3" s="20">
-        <f t="shared" ref="D3:D21" si="1">$G$4+$I$4*A3</f>
-        <v>6.9402041488310834E-2</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="3"/>
+      <c r="D3" s="14">
+        <f t="shared" ref="D3:D21" si="1">B3-C3</f>
+        <v>8.629441624365547E-4</v>
+      </c>
+      <c r="E3" s="9">
+        <f t="shared" ref="E3:E21" si="2">$K$4+$M$4*A3</f>
+        <v>8.2958288770053484E-2</v>
+      </c>
+      <c r="F3" s="12">
+        <f t="shared" ref="F3:F21" si="3">B3-E3</f>
+        <v>-2.2958288770053487E-2</v>
+      </c>
+      <c r="G3" s="9">
+        <f t="shared" ref="G3:G21" si="4">$K$6+$M$6*A3</f>
+        <v>6.9477890496516814E-2</v>
+      </c>
+      <c r="H3" s="12">
+        <f t="shared" ref="H3:H21" si="5">C3-G3</f>
+        <v>-1.0340834658953371E-2</v>
+      </c>
+      <c r="J3" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="31"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="12">
+    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
         <v>14</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="6">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="C4" s="20">
+      <c r="C4" s="9">
         <f t="shared" si="0"/>
         <v>6.8812182741116751E-2</v>
       </c>
-      <c r="D4" s="20">
+      <c r="D4" s="14">
         <f t="shared" si="1"/>
-        <v>8.529766216661179E-2</v>
-      </c>
-      <c r="F4" s="6" t="s">
+        <v>1.1878172588832558E-3</v>
+      </c>
+      <c r="E4" s="9">
+        <f t="shared" si="2"/>
+        <v>0.10093711229946525</v>
+      </c>
+      <c r="F4" s="12">
+        <f t="shared" si="3"/>
+        <v>-3.0937112299465247E-2</v>
+      </c>
+      <c r="G4" s="9">
+        <f t="shared" si="4"/>
+        <v>8.5433320398396073E-2</v>
+      </c>
+      <c r="H4" s="12">
+        <f t="shared" si="5"/>
+        <v>-1.6621137657279322E-2</v>
+      </c>
+      <c r="J4" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="11">
-        <f>AVERAGE(B2:B21)-I4*AVERAGE(A2:A21)</f>
-        <v>-2.5971682581494876E-2</v>
-      </c>
-      <c r="H4" s="9" t="s">
+      <c r="K4" s="19">
+        <f>AVERAGE(B2:B6,B16:B21)-M4*AVERAGE(A2:A6,A16:A21)</f>
+        <v>-2.4914652406417104E-2</v>
+      </c>
+      <c r="L4" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="10">
-        <f>SUMPRODUCT(A2:A21,B2:B21)/SUMSQ(A2:A21)</f>
-        <v>7.9478103391504764E-3</v>
+      <c r="M4" s="32">
+        <f>(SUMPRODUCT(A2:A6,B2:B6)+SUMPRODUCT(A16:A21,B16:B21))/(SUMSQ(A2:A6)+SUMSQ(A16:A21))</f>
+        <v>8.9894117647058829E-3</v>
+      </c>
+      <c r="N4" s="30">
+        <f>SUMSQ(F2:F6)+SUMSQ(F17:F21)</f>
+        <v>3.0596013605879477E-2</v>
+      </c>
+      <c r="O4" s="30">
+        <f>SUMSQ(F7:F16)</f>
+        <v>5.9786115721010072E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="12">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>16</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="6">
         <v>0.08</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="9">
         <f t="shared" si="0"/>
         <v>7.8487309644670045E-2</v>
       </c>
-      <c r="D5" s="20">
+      <c r="D5" s="14">
         <f t="shared" si="1"/>
-        <v>0.10119328284491275</v>
-      </c>
+        <v>1.512690355329957E-3</v>
+      </c>
+      <c r="E5" s="9">
+        <f t="shared" si="2"/>
+        <v>0.11891593582887702</v>
+      </c>
+      <c r="F5" s="12">
+        <f t="shared" si="3"/>
+        <v>-3.8915935828877021E-2</v>
+      </c>
+      <c r="G5" s="9">
+        <f t="shared" si="4"/>
+        <v>0.10138875030027533</v>
+      </c>
+      <c r="H5" s="12">
+        <f t="shared" si="5"/>
+        <v>-2.2901440655605287E-2</v>
+      </c>
+      <c r="J5" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="27"/>
+      <c r="N5" s="31"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
+    <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
         <v>18</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="6">
         <v>0.1</v>
       </c>
-      <c r="C6" s="20">
+      <c r="C6" s="9">
         <f t="shared" si="0"/>
         <v>8.8162436548223339E-2</v>
       </c>
-      <c r="D6" s="20">
+      <c r="D6" s="14">
         <f t="shared" si="1"/>
-        <v>0.11708890352321369</v>
+        <v>1.1837563451776667E-2</v>
+      </c>
+      <c r="E6" s="9">
+        <f t="shared" si="2"/>
+        <v>0.13689475935828879</v>
+      </c>
+      <c r="F6" s="12">
+        <f t="shared" si="3"/>
+        <v>-3.6894759358288787E-2</v>
+      </c>
+      <c r="G6" s="9">
+        <f t="shared" si="4"/>
+        <v>0.11734418020215459</v>
+      </c>
+      <c r="H6" s="12">
+        <f t="shared" si="5"/>
+        <v>-2.9181743653931252E-2</v>
+      </c>
+      <c r="J6" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" s="19">
+        <f>AVERAGE(B4:B23)-M6*AVERAGE(A4:A23)</f>
+        <v>-2.6254688914758767E-2</v>
+      </c>
+      <c r="L6" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="M6" s="24">
+        <f>SUMPRODUCT(A4:A23,B4:B23)/SUMSQ(A4:A23)</f>
+        <v>7.9777149509396312E-3</v>
+      </c>
+      <c r="N6" s="30">
+        <f>SUMSQ(H2:H21)</f>
+        <v>0.14737571753566764</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="12">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>20</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="6">
         <v>0.1</v>
       </c>
-      <c r="C7" s="20">
+      <c r="C7" s="9">
         <f t="shared" si="0"/>
         <v>9.7837563451776646E-2</v>
       </c>
-      <c r="D7" s="20">
+      <c r="D7" s="14">
         <f t="shared" si="1"/>
-        <v>0.13298452420151466</v>
+        <v>2.1624365482233593E-3</v>
+      </c>
+      <c r="E7" s="9">
+        <f t="shared" si="2"/>
+        <v>0.15487358288770056</v>
+      </c>
+      <c r="F7" s="12">
+        <f t="shared" si="3"/>
+        <v>-5.4873582887700556E-2</v>
+      </c>
+      <c r="G7" s="9">
+        <f t="shared" si="4"/>
+        <v>0.13329961010403385</v>
+      </c>
+      <c r="H7" s="12">
+        <f t="shared" si="5"/>
+        <v>-3.5462046652257204E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="12">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>22</v>
       </c>
-      <c r="B8" s="17">
+      <c r="B8" s="6">
         <v>0.11</v>
       </c>
-      <c r="C8" s="20">
+      <c r="C8" s="9">
         <f t="shared" si="0"/>
         <v>0.10751269035532994</v>
       </c>
-      <c r="D8" s="20">
+      <c r="D8" s="14">
         <f t="shared" si="1"/>
-        <v>0.1488801448798156</v>
+        <v>2.4873096446700604E-3</v>
+      </c>
+      <c r="E8" s="9">
+        <f t="shared" si="2"/>
+        <v>0.17285240641711233</v>
+      </c>
+      <c r="F8" s="12">
+        <f t="shared" si="3"/>
+        <v>-6.285240641711233E-2</v>
+      </c>
+      <c r="G8" s="9">
+        <f t="shared" si="4"/>
+        <v>0.14925504000591311</v>
+      </c>
+      <c r="H8" s="12">
+        <f t="shared" si="5"/>
+        <v>-4.1742349650583169E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="12">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <v>24</v>
       </c>
-      <c r="B9" s="17">
+      <c r="B9" s="6">
         <v>0.12</v>
       </c>
-      <c r="C9" s="20">
+      <c r="C9" s="9">
         <f t="shared" si="0"/>
         <v>0.11718781725888323</v>
       </c>
-      <c r="D9" s="20">
+      <c r="D9" s="14">
         <f t="shared" si="1"/>
-        <v>0.16477576555811654</v>
+        <v>2.8121827411167616E-3</v>
+      </c>
+      <c r="E9" s="9">
+        <f t="shared" si="2"/>
+        <v>0.19083122994652407</v>
+      </c>
+      <c r="F9" s="12">
+        <f t="shared" si="3"/>
+        <v>-7.0831229946524077E-2</v>
+      </c>
+      <c r="G9" s="9">
+        <f t="shared" si="4"/>
+        <v>0.1652104699077924</v>
+      </c>
+      <c r="H9" s="12">
+        <f t="shared" si="5"/>
+        <v>-4.8022652648909162E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="12">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>26</v>
       </c>
-      <c r="B10" s="17">
+      <c r="B10" s="6">
         <v>0.12</v>
       </c>
-      <c r="C10" s="20">
+      <c r="C10" s="9">
         <f t="shared" si="0"/>
         <v>0.12686294416243654</v>
       </c>
-      <c r="D10" s="20">
+      <c r="D10" s="14">
         <f t="shared" si="1"/>
-        <v>0.18067138623641751</v>
+        <v>-6.8629441624365461E-3</v>
+      </c>
+      <c r="E10" s="9">
+        <f t="shared" si="2"/>
+        <v>0.20881005347593584</v>
+      </c>
+      <c r="F10" s="12">
+        <f t="shared" si="3"/>
+        <v>-8.8810053475935846E-2</v>
+      </c>
+      <c r="G10" s="9">
+        <f t="shared" si="4"/>
+        <v>0.18116589980967165</v>
+      </c>
+      <c r="H10" s="12">
+        <f t="shared" si="5"/>
+        <v>-5.4302955647235113E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="12">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
         <v>28</v>
       </c>
-      <c r="B11" s="17">
+      <c r="B11" s="6">
         <v>0.12</v>
       </c>
-      <c r="C11" s="20">
+      <c r="C11" s="9">
         <f t="shared" si="0"/>
         <v>0.13653807106598986</v>
       </c>
-      <c r="D11" s="20">
+      <c r="D11" s="14">
         <f t="shared" si="1"/>
-        <v>0.19656700691471846</v>
+        <v>-1.6538071065989868E-2</v>
+      </c>
+      <c r="E11" s="9">
+        <f t="shared" si="2"/>
+        <v>0.22678887700534761</v>
+      </c>
+      <c r="F11" s="12">
+        <f t="shared" si="3"/>
+        <v>-0.10678887700534762</v>
+      </c>
+      <c r="G11" s="9">
+        <f t="shared" si="4"/>
+        <v>0.19712132971155091</v>
+      </c>
+      <c r="H11" s="12">
+        <f t="shared" si="5"/>
+        <v>-6.058325864556105E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="12">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
         <v>30</v>
       </c>
-      <c r="B12" s="17">
+      <c r="B12" s="6">
         <v>0.18</v>
       </c>
-      <c r="C12" s="20">
+      <c r="C12" s="9">
         <f t="shared" si="0"/>
         <v>0.14621319796954313</v>
       </c>
-      <c r="D12" s="20">
+      <c r="D12" s="14">
         <f t="shared" si="1"/>
-        <v>0.21246262759301943</v>
+        <v>3.3786802030456864E-2</v>
+      </c>
+      <c r="E12" s="9">
+        <f t="shared" si="2"/>
+        <v>0.24476770053475938</v>
+      </c>
+      <c r="F12" s="12">
+        <f t="shared" si="3"/>
+        <v>-6.4767700534759387E-2</v>
+      </c>
+      <c r="G12" s="9">
+        <f t="shared" si="4"/>
+        <v>0.21307675961343017</v>
+      </c>
+      <c r="H12" s="12">
+        <f t="shared" si="5"/>
+        <v>-6.6863561643887043E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="12">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
         <v>32</v>
       </c>
-      <c r="B13" s="17">
+      <c r="B13" s="6">
         <v>0.2</v>
       </c>
-      <c r="C13" s="20">
+      <c r="C13" s="9">
         <f t="shared" si="0"/>
         <v>0.15588832487309645</v>
       </c>
-      <c r="D13" s="20">
+      <c r="D13" s="14">
         <f t="shared" si="1"/>
-        <v>0.22835824827132037</v>
+        <v>4.411167512690356E-2</v>
+      </c>
+      <c r="E13" s="9">
+        <f t="shared" si="2"/>
+        <v>0.26274652406417115</v>
+      </c>
+      <c r="F13" s="12">
+        <f t="shared" si="3"/>
+        <v>-6.2746524064171139E-2</v>
+      </c>
+      <c r="G13" s="9">
+        <f t="shared" si="4"/>
+        <v>0.22903218951530943</v>
+      </c>
+      <c r="H13" s="12">
+        <f t="shared" si="5"/>
+        <v>-7.314386464221298E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="12">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
         <v>34</v>
       </c>
-      <c r="B14" s="17">
+      <c r="B14" s="6">
         <v>0.21</v>
       </c>
-      <c r="C14" s="20">
+      <c r="C14" s="9">
         <f t="shared" si="0"/>
         <v>0.16556345177664972</v>
       </c>
-      <c r="D14" s="20">
+      <c r="D14" s="14">
         <f t="shared" si="1"/>
-        <v>0.24425386894962134</v>
+        <v>4.4436548223350275E-2</v>
+      </c>
+      <c r="E14" s="9">
+        <f t="shared" si="2"/>
+        <v>0.28072534759358292</v>
+      </c>
+      <c r="F14" s="12">
+        <f t="shared" si="3"/>
+        <v>-7.0725347593582927E-2</v>
+      </c>
+      <c r="G14" s="9">
+        <f t="shared" si="4"/>
+        <v>0.24498761941718869</v>
+      </c>
+      <c r="H14" s="12">
+        <f t="shared" si="5"/>
+        <v>-7.9424167640538973E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="12">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
         <v>36</v>
       </c>
-      <c r="B15" s="17">
+      <c r="B15" s="6">
         <v>0.21</v>
       </c>
-      <c r="C15" s="20">
+      <c r="C15" s="9">
         <f t="shared" si="0"/>
         <v>0.17523857868020304</v>
       </c>
-      <c r="D15" s="20">
+      <c r="D15" s="14">
         <f t="shared" si="1"/>
-        <v>0.26014948962792228</v>
+        <v>3.4761421319796953E-2</v>
+      </c>
+      <c r="E15" s="9">
+        <f t="shared" si="2"/>
+        <v>0.29870417112299469</v>
+      </c>
+      <c r="F15" s="12">
+        <f t="shared" si="3"/>
+        <v>-8.8704171122994696E-2</v>
+      </c>
+      <c r="G15" s="9">
+        <f t="shared" si="4"/>
+        <v>0.26094304931906798</v>
+      </c>
+      <c r="H15" s="12">
+        <f t="shared" si="5"/>
+        <v>-8.5704470638864938E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="12">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
         <v>38</v>
       </c>
-      <c r="B16" s="17">
+      <c r="B16" s="6">
         <v>0.23</v>
       </c>
-      <c r="C16" s="20">
+      <c r="C16" s="9">
         <f t="shared" si="0"/>
         <v>0.18491370558375636</v>
       </c>
-      <c r="D16" s="20">
+      <c r="D16" s="14">
         <f t="shared" si="1"/>
-        <v>0.27604511030622325</v>
+        <v>4.508629441624365E-2</v>
+      </c>
+      <c r="E16" s="9">
+        <f t="shared" si="2"/>
+        <v>0.31668299465240646</v>
+      </c>
+      <c r="F16" s="12">
+        <f t="shared" si="3"/>
+        <v>-8.6682994652406448E-2</v>
+      </c>
+      <c r="G16" s="9">
+        <f t="shared" si="4"/>
+        <v>0.27689847922094724</v>
+      </c>
+      <c r="H16" s="12">
+        <f t="shared" si="5"/>
+        <v>-9.1984773637190875E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="12">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
         <v>40</v>
       </c>
-      <c r="B17" s="17">
+      <c r="B17" s="6">
         <v>0.28000000000000003</v>
       </c>
-      <c r="C17" s="20">
+      <c r="C17" s="9">
         <f t="shared" si="0"/>
         <v>0.19458883248730963</v>
       </c>
-      <c r="D17" s="20">
+      <c r="D17" s="14">
         <f t="shared" si="1"/>
-        <v>0.29194073098452422</v>
+        <v>8.54111675126904E-2</v>
+      </c>
+      <c r="E17" s="9">
+        <f t="shared" si="2"/>
+        <v>0.33466181818181823</v>
+      </c>
+      <c r="F17" s="12">
+        <f t="shared" si="3"/>
+        <v>-5.46618181818182E-2</v>
+      </c>
+      <c r="G17" s="9">
+        <f t="shared" si="4"/>
+        <v>0.29285390912282649</v>
+      </c>
+      <c r="H17" s="12">
+        <f t="shared" si="5"/>
+        <v>-9.8265076635516868E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="12">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
         <v>44</v>
       </c>
-      <c r="B18" s="17">
+      <c r="B18" s="6">
         <v>0.4</v>
       </c>
-      <c r="C18" s="20">
+      <c r="C18" s="9">
         <f t="shared" si="0"/>
         <v>0.21393908629441621</v>
       </c>
-      <c r="D18" s="20">
+      <c r="D18" s="14">
         <f t="shared" si="1"/>
-        <v>0.32373197234112605</v>
+        <v>0.18606091370558381</v>
+      </c>
+      <c r="E18" s="9">
+        <f t="shared" si="2"/>
+        <v>0.37061946524064177</v>
+      </c>
+      <c r="F18" s="12">
+        <f t="shared" si="3"/>
+        <v>2.9380534759358257E-2</v>
+      </c>
+      <c r="G18" s="9">
+        <f t="shared" si="4"/>
+        <v>0.32476476892658501</v>
+      </c>
+      <c r="H18" s="12">
+        <f t="shared" si="5"/>
+        <v>-0.1108256826321688</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="12">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
         <v>50</v>
       </c>
-      <c r="B19" s="17">
+      <c r="B19" s="6">
         <v>0.5</v>
       </c>
-      <c r="C19" s="20">
+      <c r="C19" s="9">
         <f t="shared" si="0"/>
         <v>0.24296446700507612</v>
       </c>
-      <c r="D19" s="20">
+      <c r="D19" s="14">
         <f t="shared" si="1"/>
-        <v>0.37141883437602896</v>
+        <v>0.25703553299492388</v>
+      </c>
+      <c r="E19" s="9">
+        <f t="shared" si="2"/>
+        <v>0.42455593582887702</v>
+      </c>
+      <c r="F19" s="12">
+        <f t="shared" si="3"/>
+        <v>7.5444064171122982E-2</v>
+      </c>
+      <c r="G19" s="9">
+        <f t="shared" si="4"/>
+        <v>0.37263105863222279</v>
+      </c>
+      <c r="H19" s="12">
+        <f t="shared" si="5"/>
+        <v>-0.12966659162714667</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="12">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
         <v>60</v>
       </c>
-      <c r="B20" s="17">
+      <c r="B20" s="6">
         <v>0.6</v>
       </c>
-      <c r="C20" s="20">
+      <c r="C20" s="9">
         <f t="shared" si="0"/>
         <v>0.29134010152284262</v>
       </c>
-      <c r="D20" s="20">
+      <c r="D20" s="14">
         <f t="shared" si="1"/>
-        <v>0.4508969377675337</v>
+        <v>0.30865989847715736</v>
+      </c>
+      <c r="E20" s="9">
+        <f t="shared" si="2"/>
+        <v>0.51445005347593586</v>
+      </c>
+      <c r="F20" s="12">
+        <f t="shared" si="3"/>
+        <v>8.5549946524064113E-2</v>
+      </c>
+      <c r="G20" s="9">
+        <f t="shared" si="4"/>
+        <v>0.45240820814161908</v>
+      </c>
+      <c r="H20" s="12">
+        <f t="shared" si="5"/>
+        <v>-0.16106810661877646</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="13">
+    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
         <v>70</v>
       </c>
-      <c r="B21" s="18">
+      <c r="B21" s="7">
         <v>0.7</v>
       </c>
-      <c r="C21" s="20">
+      <c r="C21" s="10">
         <f t="shared" si="0"/>
         <v>0.33971573604060912</v>
       </c>
-      <c r="D21" s="20">
+      <c r="D21" s="15">
         <f t="shared" si="1"/>
-        <v>0.53037504115903855</v>
+        <v>0.36028426395939084</v>
+      </c>
+      <c r="E21" s="9">
+        <f t="shared" si="2"/>
+        <v>0.60434417112299466</v>
+      </c>
+      <c r="F21" s="12">
+        <f t="shared" si="3"/>
+        <v>9.56558288770053E-2</v>
+      </c>
+      <c r="G21" s="9">
+        <f t="shared" si="4"/>
+        <v>0.53218535765101538</v>
+      </c>
+      <c r="H21" s="1">
+        <f t="shared" si="5"/>
+        <v>-0.19246962161040626</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="16"/>
+      <c r="D22" s="17">
+        <f>SUMSQ(D2:D21)</f>
+        <v>0.34184404545337421</v>
+      </c>
+      <c r="F22" s="17">
+        <f>SUMSQ(F2:F21)</f>
+        <v>9.0382129326889563E-2</v>
+      </c>
+      <c r="H22" s="17">
+        <f>SUMSQ(H2:H21)</f>
+        <v>0.14737571753566764</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="F1:I1"/>
+  <mergeCells count="4">
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="J5:M5"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>